<commit_message>
support for converting excel formated dates to string
</commit_message>
<xml_diff>
--- a/specs/test.xlsx
+++ b/specs/test.xlsx
@@ -16,30 +16,31 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt formatCode="GENERAL" numFmtId="164"/>
+    <numFmt formatCode="M/D/YYYY" numFmtId="165"/>
   </numFmts>
   <fonts count="4">
     <font>
+      <name val="Arial"/>
+      <charset val="1"/>
+      <family val="2"/>
       <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
-      <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
+      <sz val="10"/>
     </font>
     <font>
-      <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
+      <sz val="10"/>
     </font>
     <font>
-      <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
+      <sz val="10"/>
     </font>
   </fonts>
   <fills count="2">
@@ -84,8 +85,12 @@
     <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="42"/>
     <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="9"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0">
+      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="165" xfId="0">
       <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
       <protection hidden="false" locked="true"/>
     </xf>
@@ -106,10 +111,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:KN115"/>
+  <dimension ref="A1:KN116"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="A1" activeCellId="0" pane="topLeft" sqref="A1"/>
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A94" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
+      <selection activeCell="D117" activeCellId="0" pane="topLeft" sqref="D117"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -1586,6 +1591,20 @@
         <v>115</v>
       </c>
     </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.85" outlineLevel="0" r="116">
+      <c r="A116" s="1" t="n">
+        <v>41200</v>
+      </c>
+      <c r="B116" s="1" t="n">
+        <v>41200.0124772222</v>
+      </c>
+      <c r="C116" s="1" t="n">
+        <v>41091.8880671296</v>
+      </c>
+      <c r="D116" s="1" t="n">
+        <v>41091.8881134259</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
dullard now reads cell formatting from stylesheet and allows for user defined formats
</commit_message>
<xml_diff>
--- a/specs/test.xlsx
+++ b/specs/test.xlsx
@@ -14,11 +14,20 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
+  <si>
+    <t>teststring</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt formatCode="GENERAL" numFmtId="164"/>
-    <numFmt formatCode="M/D/YYYY" numFmtId="165"/>
+    <numFmt formatCode="M/D/YY" numFmtId="165"/>
+    <numFmt formatCode="M/D/YYYY" numFmtId="166"/>
   </numFmts>
   <fonts count="4">
     <font>
@@ -85,12 +94,16 @@
     <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="42"/>
     <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="9"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0">
       <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
       <protection hidden="false" locked="true"/>
     </xf>
     <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="165" xfId="0">
+      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="166" xfId="0">
       <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
       <protection hidden="false" locked="true"/>
     </xf>
@@ -111,10 +124,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:KN116"/>
+  <dimension ref="A1:KN117"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A94" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="D117" activeCellId="0" pane="topLeft" sqref="D117"/>
+      <selection activeCell="F106" activeCellId="0" pane="topLeft" sqref="F106"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -1605,6 +1618,23 @@
         <v>41091.8881134259</v>
       </c>
     </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="117">
+      <c r="A117" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="B117" s="2" t="n">
+        <v>41200</v>
+      </c>
+      <c r="C117" s="2" t="n">
+        <v>41200.0124772222</v>
+      </c>
+      <c r="D117" s="2" t="n">
+        <v>41091.8880671296</v>
+      </c>
+      <c r="E117" s="2" t="n">
+        <v>41091.8881134259</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>